<commit_message>
penambahan add account algoritma
</commit_message>
<xml_diff>
--- a/static/doc/excel/data_karyawan.xlsx
+++ b/static/doc/excel/data_karyawan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Karyawan" sheetId="1" state="visible" r:id="rId1"/>
@@ -67,7 +67,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -76,26 +76,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -117,31 +108,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -262,6 +252,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="476250" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -564,265 +579,324 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="3" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="28" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="22" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
-    <col width="9" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
-    <col width="27" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
-    <col width="17" bestFit="1" customWidth="1" style="4" min="6" max="6"/>
-    <col width="12" bestFit="1" customWidth="1" style="4" min="7" max="7"/>
-    <col width="17" bestFit="1" customWidth="1" style="4" min="8" max="8"/>
-    <col width="16" bestFit="1" customWidth="1" style="4" min="9" max="9"/>
-    <col width="20" bestFit="1" customWidth="1" style="5" min="10" max="10"/>
-    <col width="20" bestFit="1" customWidth="1" style="5" min="11" max="11"/>
-    <col width="17" bestFit="1" customWidth="1" style="5" min="12" max="12"/>
-    <col width="20" bestFit="1" customWidth="1" style="5" min="13" max="13"/>
-    <col width="6" bestFit="1" customWidth="1" style="5" min="14" max="14"/>
-    <col width="12" bestFit="1" customWidth="1" style="5" min="15" max="15"/>
+    <col width="3" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="28" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="22" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="9" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="27" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
+    <col width="17" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col width="12" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
+    <col width="17" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
+    <col width="16" bestFit="1" customWidth="1" style="1" min="9" max="9"/>
+    <col width="20" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
+    <col width="20" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
+    <col width="17" bestFit="1" customWidth="1" style="2" min="12" max="12"/>
+    <col width="20" bestFit="1" customWidth="1" style="2" min="13" max="13"/>
+    <col width="6" bestFit="1" customWidth="1" style="2" min="14" max="14"/>
+    <col width="6" bestFit="1" customWidth="1" style="2" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="5" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Data Karyawan PT Winnicode Garuda Teknologi</t>
         </is>
       </c>
-      <c r="B1" s="7" t="n"/>
-      <c r="C1" s="7" t="n"/>
-      <c r="D1" s="7" t="n"/>
-      <c r="E1" s="7" t="n"/>
-      <c r="F1" s="7" t="n"/>
-      <c r="G1" s="7" t="n"/>
-      <c r="H1" s="7" t="n"/>
-      <c r="I1" s="7" t="n"/>
-      <c r="J1" s="7" t="n"/>
-      <c r="K1" s="7" t="n"/>
-      <c r="L1" s="7" t="n"/>
-      <c r="M1" s="7" t="n"/>
-      <c r="N1" s="7" t="n"/>
-      <c r="O1" s="7" t="n"/>
     </row>
     <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Nama</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>Departement</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
         <is>
           <t>Jobs</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>NIK</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Foto Profil</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="H2" s="6" t="inlineStr">
         <is>
           <t>Tempat Lahir</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="I2" s="6" t="inlineStr">
         <is>
           <t>Tanggal Lahir</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>Tanggal Mulai Kerja</t>
         </is>
       </c>
-      <c r="K2" s="3" t="inlineStr">
+      <c r="K2" s="5" t="inlineStr">
         <is>
           <t>Tanggal Akhir Kerja</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="L2" s="4" t="inlineStr">
         <is>
           <t>Waktu Awal Kerja</t>
         </is>
       </c>
-      <c r="M2" s="3" t="inlineStr">
+      <c r="M2" s="5" t="inlineStr">
         <is>
           <t>Waktu Selesai kerja</t>
         </is>
       </c>
-      <c r="N2" s="2" t="inlineStr">
+      <c r="N2" s="4" t="inlineStr">
         <is>
           <t>Hadir</t>
         </is>
       </c>
-      <c r="O2" s="3" t="inlineStr">
+      <c r="O2" s="5" t="inlineStr">
+        <is>
+          <t>Telat</t>
+        </is>
+      </c>
+      <c r="P2" s="4" t="inlineStr">
         <is>
           <t>Tidak Hadir</t>
+        </is>
+      </c>
+      <c r="Q2" s="5" t="inlineStr">
+        <is>
+          <t>Cuti</t>
         </is>
       </c>
     </row>
     <row r="3" ht="44" customHeight="1">
-      <c r="A3" s="8" t="n">
+      <c r="A3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="inlineStr">
+      <c r="B3" s="7" t="inlineStr">
         <is>
           <t>Salahudin Kholik Prasetyono</t>
         </is>
       </c>
-      <c r="C3" s="8" t="inlineStr">
+      <c r="C3" s="7" t="inlineStr">
         <is>
           <t>Fullstack Developer</t>
         </is>
       </c>
-      <c r="D3" s="8" t="inlineStr">
+      <c r="D3" s="7" t="inlineStr">
         <is>
           <t>Magang</t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr">
+      <c r="E3" s="7" t="inlineStr">
         <is>
           <t>salahudinkoliq12@gmail.com</t>
         </is>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="7" t="n">
         <v>3216071205030011</v>
       </c>
-      <c r="G3" s="9" t="inlineStr">
+      <c r="G3" s="8" t="inlineStr">
         <is>
           <t>img/user/unnamed.jpg</t>
         </is>
       </c>
-      <c r="H3" s="8" t="inlineStr">
+      <c r="H3" s="7" t="inlineStr">
         <is>
           <t>Kabupaten Bekasi</t>
         </is>
       </c>
-      <c r="I3" s="8" t="inlineStr">
+      <c r="I3" s="7" t="inlineStr">
         <is>
           <t>12 may 2004</t>
         </is>
       </c>
-      <c r="J3" s="8" t="inlineStr">
+      <c r="J3" s="7" t="inlineStr">
         <is>
           <t>15 september 2024</t>
         </is>
       </c>
-      <c r="K3" s="8" t="inlineStr">
+      <c r="K3" s="7" t="inlineStr">
         <is>
           <t>31 december 2024</t>
         </is>
       </c>
-      <c r="L3" s="8" t="inlineStr">
+      <c r="L3" s="7" t="inlineStr">
         <is>
           <t>08.00</t>
         </is>
       </c>
-      <c r="M3" s="8" t="inlineStr">
+      <c r="M3" s="7" t="inlineStr">
         <is>
           <t>18.00</t>
         </is>
       </c>
-      <c r="N3" s="8" t="n">
+      <c r="N3" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="O3" s="8" t="n">
-        <v>14</v>
+      <c r="O3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="44" customHeight="1">
-      <c r="A4" s="8" t="n">
+      <c r="A4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="inlineStr">
+      <c r="B4" s="7" t="inlineStr">
         <is>
           <t>Salahudin Kholik Prasetonos</t>
         </is>
       </c>
-      <c r="C4" s="8" t="inlineStr">
+      <c r="C4" s="7" t="inlineStr">
         <is>
           <t>Web Developer Laravel</t>
         </is>
       </c>
-      <c r="D4" s="8" t="inlineStr">
+      <c r="D4" s="7" t="inlineStr">
         <is>
           <t>Karyawan</t>
         </is>
       </c>
-      <c r="E4" s="8" t="inlineStr">
+      <c r="E4" s="7" t="inlineStr">
         <is>
           <t>salahudinkoliq10@gmail.com</t>
         </is>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="7" t="n">
         <v>3216071205030011</v>
       </c>
-      <c r="G4" s="9" t="inlineStr">
+      <c r="G4" s="8" t="inlineStr">
         <is>
           <t>img/user/campuscoder-poster-2.png</t>
         </is>
       </c>
-      <c r="H4" s="8" t="inlineStr">
+      <c r="H4" s="7" t="inlineStr">
         <is>
           <t>Bekasi</t>
         </is>
       </c>
-      <c r="I4" s="8" t="inlineStr">
+      <c r="I4" s="7" t="inlineStr">
         <is>
           <t>12 january 2003</t>
         </is>
       </c>
-      <c r="J4" s="8" t="inlineStr">
+      <c r="J4" s="7" t="inlineStr">
         <is>
           <t>27 september 2024</t>
         </is>
       </c>
-      <c r="K4" s="8" t="inlineStr">
+      <c r="K4" s="7" t="inlineStr">
         <is>
           <t>31 december 2024</t>
         </is>
       </c>
-      <c r="L4" s="8" t="inlineStr">
+      <c r="L4" s="7" t="inlineStr">
         <is>
           <t>08.00</t>
         </is>
       </c>
-      <c r="M4" s="8" t="inlineStr">
+      <c r="M4" s="7" t="inlineStr">
         <is>
           <t>16.00</t>
         </is>
       </c>
-      <c r="N4" s="8" t="n">
-        <v>22</v>
-      </c>
-      <c r="O4" s="8" t="n">
-        <v>12</v>
+      <c r="N4" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="O4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="44" customHeight="1">
+      <c r="A5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Bonardi</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>Fullstack Developer</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>Magang</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>bonardi@gmail.com</t>
+        </is>
+      </c>
+      <c r="F5" s="7" t="inlineStr"/>
+      <c r="G5" s="8" t="inlineStr">
+        <is>
+          <t>img/default/user.png</t>
+        </is>
+      </c>
+      <c r="H5" s="7" t="inlineStr"/>
+      <c r="I5" s="7" t="inlineStr"/>
+      <c r="J5" s="7" t="inlineStr"/>
+      <c r="K5" s="7" t="inlineStr"/>
+      <c r="L5" s="7" t="inlineStr"/>
+      <c r="M5" s="7" t="inlineStr"/>
+      <c r="N5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
melakukan custom hasil export dari datatables
</commit_message>
<xml_diff>
--- a/static/doc/excel/data_karyawan.xlsx
+++ b/static/doc/excel/data_karyawan.xlsx
@@ -18,13 +18,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -36,15 +43,16 @@
     <font>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <color rgb="FFFF66C4"/>
-      <sz val="16"/>
+      <b val="1"/>
+      <color rgb="FFFF3399"/>
+      <sz val="14"/>
     </font>
     <font>
       <name val="Times"/>
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -53,8 +61,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF66C4"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
       </patternFill>
     </fill>
   </fills>
@@ -99,21 +116,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -129,7 +161,7 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>5</col>
+      <col>6</col>
       <colOff>0</colOff>
       <row>2</row>
       <rowOff>0</rowOff>
@@ -154,7 +186,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>5</col>
+      <col>6</col>
       <colOff>0</colOff>
       <row>3</row>
       <rowOff>0</rowOff>
@@ -179,7 +211,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>5</col>
+      <col>6</col>
       <colOff>0</colOff>
       <row>4</row>
       <rowOff>0</rowOff>
@@ -192,6 +224,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>5</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="476250" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -494,156 +551,423 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="4" customWidth="1" style="1" min="1" max="1"/>
-    <col width="32" customWidth="1" style="1" min="2" max="2"/>
-    <col width="28" customWidth="1" style="1" min="3" max="3"/>
-    <col width="13" customWidth="1" style="1" min="4" max="4"/>
-    <col width="7" customWidth="1" style="1" min="5" max="5"/>
-    <col width="13" customWidth="1" style="1" min="6" max="6"/>
+    <col width="4" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="29" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="23" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="10" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="29" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
+    <col width="18" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col width="13" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
+    <col width="18" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
+    <col width="17" bestFit="1" customWidth="1" style="1" min="9" max="9"/>
+    <col width="21" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
+    <col width="21" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
+    <col width="18" bestFit="1" customWidth="1" style="2" min="12" max="12"/>
+    <col width="21" bestFit="1" customWidth="1" style="2" min="13" max="13"/>
+    <col width="7" bestFit="1" customWidth="1" style="2" min="14" max="14"/>
+    <col width="7" bestFit="1" customWidth="1" style="2" min="15" max="15"/>
+    <col width="13" customWidth="1" min="16" max="16"/>
+    <col width="6" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32.5" customHeight="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Data Admin PT Winnicode Garuda Teknologi</t>
+    <row r="1" ht="26" customHeight="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>Data Karyawan PT Winnicode Garuda Teknologi</t>
         </is>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>Nama</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>Departement</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Jobs</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Departement</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>Jobs</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>NIK</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
         <is>
           <t>Foto Profil</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>Tempat Lahir</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>Tanggal Lahir</t>
+        </is>
+      </c>
+      <c r="J2" s="6" t="inlineStr">
+        <is>
+          <t>Tanggal Mulai Kerja</t>
+        </is>
+      </c>
+      <c r="K2" s="7" t="inlineStr">
+        <is>
+          <t>Tanggal Akhir Kerja</t>
+        </is>
+      </c>
+      <c r="L2" s="6" t="inlineStr">
+        <is>
+          <t>Waktu Awal Kerja</t>
+        </is>
+      </c>
+      <c r="M2" s="7" t="inlineStr">
+        <is>
+          <t>Waktu Selesai kerja</t>
+        </is>
+      </c>
+      <c r="N2" s="6" t="inlineStr">
+        <is>
+          <t>Hadir</t>
+        </is>
+      </c>
+      <c r="O2" s="7" t="inlineStr">
+        <is>
+          <t>Telat</t>
+        </is>
+      </c>
+      <c r="P2" s="3" t="inlineStr">
+        <is>
+          <t>Tidak Hadir</t>
+        </is>
+      </c>
+      <c r="Q2" s="4" t="inlineStr">
+        <is>
+          <t>Cuti</t>
         </is>
       </c>
     </row>
     <row r="3" ht="44" customHeight="1">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>Salahudin kholik Prasetonosasa</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>admin2@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>Superuser</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>img/default/user.png</t>
-        </is>
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>Salahudin Kholik Prasetyono</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>Fullstack Developer</t>
+        </is>
+      </c>
+      <c r="D3" s="9" t="inlineStr">
+        <is>
+          <t>Magang</t>
+        </is>
+      </c>
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>salahudinkoliq12@gmail.com</t>
+        </is>
+      </c>
+      <c r="F3" s="9" t="n">
+        <v>3216071205030011</v>
+      </c>
+      <c r="G3" s="10" t="inlineStr">
+        <is>
+          <t>img/user/unnamed.jpg</t>
+        </is>
+      </c>
+      <c r="H3" s="9" t="inlineStr">
+        <is>
+          <t>Kabupaten Bekasi</t>
+        </is>
+      </c>
+      <c r="I3" s="9" t="inlineStr">
+        <is>
+          <t>12 may 2004</t>
+        </is>
+      </c>
+      <c r="J3" s="9" t="inlineStr">
+        <is>
+          <t>15 september 2024</t>
+        </is>
+      </c>
+      <c r="K3" s="9" t="inlineStr">
+        <is>
+          <t>31 december 2024</t>
+        </is>
+      </c>
+      <c r="L3" s="9" t="inlineStr">
+        <is>
+          <t>08.00</t>
+        </is>
+      </c>
+      <c r="M3" s="9" t="inlineStr">
+        <is>
+          <t>18.00</t>
+        </is>
+      </c>
+      <c r="N3" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="O3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" s="9" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" ht="44" customHeight="1">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Salahudin kholik Prasetono</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>Salahudin Kholik Prasetonos</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>Web Developer Laravel</t>
+        </is>
+      </c>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t>Karyawan</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="inlineStr">
         <is>
           <t>salahudinkoliq10@gmail.com</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Mentor</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>img/default/user.png</t>
-        </is>
+      <c r="F4" s="9" t="n">
+        <v>3216071205030011</v>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>img/user/campuscoder-poster-2.png</t>
+        </is>
+      </c>
+      <c r="H4" s="9" t="inlineStr">
+        <is>
+          <t>Bekasis</t>
+        </is>
+      </c>
+      <c r="I4" s="9" t="inlineStr">
+        <is>
+          <t>12 january 2003</t>
+        </is>
+      </c>
+      <c r="J4" s="9" t="inlineStr">
+        <is>
+          <t>27 september 2024</t>
+        </is>
+      </c>
+      <c r="K4" s="9" t="inlineStr">
+        <is>
+          <t>31 december 2024</t>
+        </is>
+      </c>
+      <c r="L4" s="9" t="inlineStr">
+        <is>
+          <t>08.00</t>
+        </is>
+      </c>
+      <c r="M4" s="9" t="inlineStr">
+        <is>
+          <t>16.00</t>
+        </is>
+      </c>
+      <c r="N4" s="9" t="n">
+        <v>24</v>
+      </c>
+      <c r="O4" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="P4" s="9" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="44" customHeight="1">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>taufiqadmina</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>admin@gmail.com</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>Superuser</t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>img/user/forgot-password-concept-illustration.png</t>
-        </is>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>Bonardi</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr">
+        <is>
+          <t>Fullstack Developer</t>
+        </is>
+      </c>
+      <c r="D5" s="9" t="inlineStr">
+        <is>
+          <t>Magang</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="inlineStr">
+        <is>
+          <t>bonardi@gmail.com</t>
+        </is>
+      </c>
+      <c r="F5" s="9" t="n">
+        <v>3216071205030011</v>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>img/default/user.png</t>
+        </is>
+      </c>
+      <c r="H5" s="9" t="inlineStr">
+        <is>
+          <t>Bekasi</t>
+        </is>
+      </c>
+      <c r="I5" s="9" t="inlineStr">
+        <is>
+          <t>12 may 2003</t>
+        </is>
+      </c>
+      <c r="J5" s="9" t="inlineStr">
+        <is>
+          <t>25 october 2024</t>
+        </is>
+      </c>
+      <c r="K5" s="9" t="inlineStr">
+        <is>
+          <t>10 november 2024</t>
+        </is>
+      </c>
+      <c r="L5" s="9" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="M5" s="9" t="inlineStr">
+        <is>
+          <t>19.00</t>
+        </is>
+      </c>
+      <c r="N5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="44" customHeight="1">
+      <c r="A6" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>m taufiq</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr">
+        <is>
+          <t>Web Developer Laravel</t>
+        </is>
+      </c>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>Magang</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
+        <is>
+          <t>taufiqurrahman123@gmail.com</t>
+        </is>
+      </c>
+      <c r="F6" s="9" t="inlineStr"/>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>img/default/user.png</t>
+        </is>
+      </c>
+      <c r="H6" s="9" t="inlineStr"/>
+      <c r="I6" s="9" t="inlineStr"/>
+      <c r="J6" s="9" t="inlineStr">
+        <is>
+          <t>12 may 2003</t>
+        </is>
+      </c>
+      <c r="K6" s="9" t="inlineStr">
+        <is>
+          <t>12 may 2025</t>
+        </is>
+      </c>
+      <c r="L6" s="9" t="inlineStr">
+        <is>
+          <t>18.40</t>
+        </is>
+      </c>
+      <c r="M6" s="9" t="inlineStr">
+        <is>
+          <t>10.20</t>
+        </is>
+      </c>
+      <c r="N6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="9" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: update employee data in PDF with new entries and corrections
</commit_message>
<xml_diff>
--- a/static/doc/excel/data_karyawan.xlsx
+++ b/static/doc/excel/data_karyawan.xlsx
@@ -199,6 +199,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="476250" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -501,7 +526,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
@@ -510,10 +535,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="4" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="29" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="28" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
     <col width="23" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
     <col width="10" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
-    <col width="30" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
+    <col width="28" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
     <col width="18" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
     <col width="13" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
     <col width="14" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
@@ -628,7 +653,7 @@
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>taufiq</t>
+          <t>Salahudin Kholik Prasetono</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr">
@@ -643,32 +668,58 @@
       </c>
       <c r="E3" s="9" t="inlineStr">
         <is>
-          <t>muhammadtaufiq2097@gmail.com</t>
-        </is>
-      </c>
-      <c r="F3" s="9" t="inlineStr"/>
+          <t>salahudinkoliq10@gmail.com</t>
+        </is>
+      </c>
+      <c r="F3" s="9" t="n">
+        <v>3216071205030010</v>
+      </c>
       <c r="G3" s="10" t="inlineStr">
         <is>
-          <t>https://i.ibb.co.com/5Yd94zx/user.png</t>
-        </is>
-      </c>
-      <c r="H3" s="9" t="inlineStr"/>
-      <c r="I3" s="9" t="inlineStr"/>
-      <c r="J3" s="9" t="inlineStr"/>
-      <c r="K3" s="9" t="inlineStr"/>
-      <c r="L3" s="9" t="inlineStr"/>
-      <c r="M3" s="9" t="inlineStr"/>
+          <t>https://i.ibb.co.com/RpFz2L7x/IMG-20250705-132945-308.jpg IMG-20250705-132945-308.jpg</t>
+        </is>
+      </c>
+      <c r="H3" s="9" t="inlineStr">
+        <is>
+          <t>Bekasi</t>
+        </is>
+      </c>
+      <c r="I3" s="9" t="inlineStr">
+        <is>
+          <t>12 may 2003</t>
+        </is>
+      </c>
+      <c r="J3" s="9" t="inlineStr">
+        <is>
+          <t>12 may 2003</t>
+        </is>
+      </c>
+      <c r="K3" s="9" t="inlineStr">
+        <is>
+          <t>12 may 2026</t>
+        </is>
+      </c>
+      <c r="L3" s="9" t="inlineStr">
+        <is>
+          <t>12.30</t>
+        </is>
+      </c>
+      <c r="M3" s="9" t="inlineStr">
+        <is>
+          <t>12.55</t>
+        </is>
+      </c>
       <c r="N3" s="9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O3" s="9" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P3" s="9" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="Q3" s="9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" ht="44" customHeight="1">
@@ -677,12 +728,12 @@
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>Salahudin kholik Prasetyono</t>
+          <t>Salahudin kholik Prasetono</t>
         </is>
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>Web Developer Laravel</t>
+          <t>Fullstack Developer</t>
         </is>
       </c>
       <c r="D4" s="9" t="inlineStr">
@@ -707,34 +758,101 @@
       <c r="I4" s="9" t="inlineStr"/>
       <c r="J4" s="9" t="inlineStr">
         <is>
-          <t>27 april 2025</t>
+          <t>12 february 2025</t>
         </is>
       </c>
       <c r="K4" s="9" t="inlineStr">
         <is>
-          <t>30 april 2025</t>
+          <t>12 february 2026</t>
         </is>
       </c>
       <c r="L4" s="9" t="inlineStr">
         <is>
-          <t>01.00</t>
+          <t>12.05</t>
         </is>
       </c>
       <c r="M4" s="9" t="inlineStr">
         <is>
-          <t>12.00</t>
+          <t>14.02</t>
         </is>
       </c>
       <c r="N4" s="9" t="n">
         <v>0</v>
       </c>
       <c r="O4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" ht="44" customHeight="1">
+      <c r="A5" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>Coba1</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr">
+        <is>
+          <t>Fullstack Developer</t>
+        </is>
+      </c>
+      <c r="D5" s="9" t="inlineStr">
+        <is>
+          <t>Karyawan</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="inlineStr">
+        <is>
+          <t>coba1@gmail.com</t>
+        </is>
+      </c>
+      <c r="F5" s="9" t="n">
+        <v>3216071205030005</v>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co.com/5Yd94zx/user.png</t>
+        </is>
+      </c>
+      <c r="H5" s="9" t="inlineStr"/>
+      <c r="I5" s="9" t="inlineStr"/>
+      <c r="J5" s="9" t="inlineStr">
+        <is>
+          <t>13 july 2025</t>
+        </is>
+      </c>
+      <c r="K5" s="9" t="inlineStr">
+        <is>
+          <t>31 july 2025</t>
+        </is>
+      </c>
+      <c r="L5" s="9" t="inlineStr">
+        <is>
+          <t>18.00</t>
+        </is>
+      </c>
+      <c r="M5" s="9" t="inlineStr">
+        <is>
+          <t>22.55</t>
+        </is>
+      </c>
+      <c r="N5" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="P4" s="9" t="n">
+      <c r="O5" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" s="9" t="n">
+      <c r="P5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="9" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>